<commit_message>
support split import type
</commit_message>
<xml_diff>
--- a/Test/Input/Action.xlsx
+++ b/Test/Input/Action.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\MakeConfig.Sharp\Test\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD4C983-52E2-4846-9406-79D576D849AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E43D0F7-4387-4379-B410-AFEA2B4C7DD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,10 +468,14 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="7" max="7" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>